<commit_message>
Atorado con insertar datos
</commit_message>
<xml_diff>
--- a/Base de datos Banco azteca.xlsx
+++ b/Base de datos Banco azteca.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="124">
   <si>
     <t xml:space="preserve">Base de datos: Banco Azteca</t>
   </si>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Empleado</t>
   </si>
   <si>
-    <t xml:space="preserve">create table banco.empleado (empleado_id serial primary key, sucursal_id int references banco.sucursales(sucursal_id), departamento_id int references banco.departamentos (departamento_id), nombre_empleado text, apellido_paterno text, apellido_materno text, puesto text, salario decimal, telefono_empleado varchar(10), email_empleado text);</t>
+    <t xml:space="preserve">create table banco.empleados (empleado_id serial primary key, sucursal_id int references banco.sucursales(sucursal_id), departamento_id int references banco.departamentos (departamento_id), nombre_empleado text, apellido_paterno text, apellido_materno text, puesto text, salario decimal, telefono_empleado varchar(10), email_empleado text, password_empleado text);</t>
   </si>
   <si>
     <t xml:space="preserve">servicio_id</t>
@@ -184,6 +184,9 @@
     <t xml:space="preserve">tasa_interes</t>
   </si>
   <si>
+    <t xml:space="preserve">password_empleado</t>
+  </si>
+  <si>
     <t xml:space="preserve">comision</t>
   </si>
   <si>
@@ -377,6 +380,18 @@
   </si>
   <si>
     <t xml:space="preserve">insert into banco.tipo_tarjeta (tipo_t) values ('Guardadito'), ('Debito Azteca'), ('Guardadito Kids'), ('Debito Negocio'), ('Tarjeta de credito oro'), ('Tarjeta Azteca');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create table banco.puesto(puesto_id serial primary key, puesto text);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puesto_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert into banco.puesto (puesto) values ('Ejecutivo'), ('Asesor'), ('Atencion a clientes'), ('Gerente');</t>
   </si>
 </sst>
 </file>
@@ -386,7 +401,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +426,20 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -496,15 +525,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,7 +537,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,9 +568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>170280</xdr:colOff>
+      <xdr:colOff>169920</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -551,7 +580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5989680" y="1028880"/>
-          <a:ext cx="160920" cy="2132640"/>
+          <a:ext cx="160560" cy="2132280"/>
         </a:xfrm>
         <a:prstGeom prst="rightBracket">
           <a:avLst>
@@ -761,10 +790,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:S76"/>
+  <dimension ref="B2:M83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G57" activeCellId="0" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -950,13 +979,13 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
@@ -970,9 +999,6 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="I11" s="0"/>
-      <c r="L11" s="0"/>
-      <c r="M11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
@@ -985,12 +1011,12 @@
       <c r="I12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I13" s="5" t="s">
@@ -1013,12 +1039,12 @@
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="I14" s="5" t="s">
         <v>34</v>
       </c>
@@ -1066,7 +1092,7 @@
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="8" t="n">
+      <c r="D16" s="7" t="n">
         <v>100</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1090,7 +1116,7 @@
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="8" t="n">
+      <c r="D17" s="7" t="n">
         <v>100</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1114,7 +1140,7 @@
       <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="5" t="s">
         <v>35</v>
       </c>
@@ -1134,12 +1160,9 @@
       <c r="C19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="I19" s="0"/>
-      <c r="L19" s="0"/>
-      <c r="M19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5" t="s">
@@ -1148,7 +1171,7 @@
       <c r="C20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="I20" s="3" t="s">
@@ -1168,7 +1191,7 @@
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="I21" s="5" t="s">
@@ -1194,7 +1217,7 @@
       <c r="C22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="8"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="I22" s="5" t="s">
@@ -1216,7 +1239,7 @@
       <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="I23" s="5" t="s">
@@ -1236,7 +1259,7 @@
       <c r="C24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="8" t="n">
+      <c r="D24" s="7" t="n">
         <v>10</v>
       </c>
       <c r="E24" s="5"/>
@@ -1258,7 +1281,7 @@
       <c r="C25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="I25" s="5" t="s">
@@ -1272,8 +1295,17 @@
       <c r="M25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="I26" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>39</v>
@@ -1283,13 +1315,8 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
-      <c r="E27" s="0"/>
-      <c r="F27" s="0"/>
       <c r="I27" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>15</v>
@@ -1300,16 +1327,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -1335,7 +1362,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>11</v>
@@ -1346,18 +1373,18 @@
       </c>
       <c r="F30" s="5"/>
       <c r="I30" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
+      <c r="J30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>15</v>
@@ -1392,7 +1419,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>11</v>
@@ -1414,7 +1441,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>11</v>
@@ -1427,10 +1454,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -1460,7 +1487,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>39</v>
@@ -1471,7 +1498,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>15</v>
@@ -1491,7 +1518,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>15</v>
@@ -1500,10 +1527,10 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -1511,7 +1538,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>15</v>
@@ -1520,10 +1547,10 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -1531,7 +1558,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>24</v>
@@ -1542,7 +1569,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="I39" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J39" s="5" t="s">
         <v>15</v>
@@ -1553,7 +1580,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>24</v>
@@ -1566,25 +1593,25 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I41" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J41" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
+      <c r="J41" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="C42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
       <c r="I42" s="5" t="s">
         <v>5</v>
       </c>
@@ -1618,7 +1645,7 @@
         <v>9</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>11</v>
@@ -1631,7 +1658,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>11</v>
@@ -1642,7 +1669,7 @@
       </c>
       <c r="F44" s="5"/>
       <c r="I44" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>11</v>
@@ -1655,7 +1682,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>11</v>
@@ -1666,7 +1693,7 @@
       </c>
       <c r="F45" s="5"/>
       <c r="I45" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>15</v>
@@ -1699,7 +1726,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>24</v>
@@ -1721,16 +1748,16 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="I48" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J48" s="5" t="s">
         <v>15</v>
@@ -1741,7 +1768,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>11</v>
@@ -1765,7 +1792,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>39</v>
@@ -1774,7 +1801,7 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="I50" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>15</v>
@@ -1785,7 +1812,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>11</v>
@@ -1798,27 +1825,24 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="I52" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J52" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="O52" s="0"/>
-      <c r="R52" s="0"/>
-      <c r="S52" s="0"/>
+      <c r="J52" s="8" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>24</v>
@@ -1843,13 +1867,10 @@
       <c r="M53" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O53" s="0"/>
-      <c r="R53" s="0"/>
-      <c r="S53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I54" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J54" s="5" t="s">
         <v>11</v>
@@ -1859,22 +1880,19 @@
         <v>12</v>
       </c>
       <c r="M54" s="5"/>
-      <c r="O54" s="0"/>
-      <c r="R54" s="0"/>
-      <c r="S54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
+      <c r="C55" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
       <c r="I55" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>11</v>
@@ -1884,9 +1902,6 @@
         <v>35</v>
       </c>
       <c r="M55" s="5"/>
-      <c r="O55" s="0"/>
-      <c r="R55" s="0"/>
-      <c r="S55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="5" t="s">
@@ -1918,7 +1933,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>11</v>
@@ -1942,7 +1957,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>11</v>
@@ -1953,7 +1968,7 @@
       </c>
       <c r="F58" s="5"/>
       <c r="I58" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J58" s="5" t="s">
         <v>24</v>
@@ -1966,7 +1981,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>39</v>
@@ -1975,7 +1990,7 @@
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="I59" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J59" s="5" t="s">
         <v>39</v>
@@ -1986,7 +2001,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>24</v>
@@ -1997,7 +2012,7 @@
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="I60" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>11</v>
@@ -2010,19 +2025,19 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="I61" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
@@ -2030,13 +2045,13 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -2048,7 +2063,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>11</v>
@@ -2058,18 +2073,18 @@
         <v>35</v>
       </c>
       <c r="F63" s="5"/>
-      <c r="I63" s="10"/>
+      <c r="I63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I64" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J64" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
+      <c r="J64" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I65" s="5" t="s">
@@ -2090,16 +2105,16 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
+      <c r="C66" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
       <c r="I66" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>11</v>
@@ -2127,7 +2142,7 @@
         <v>9</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>11</v>
@@ -2140,12 +2155,12 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="11"/>
+        <v>105</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
         <v>12</v>
       </c>
@@ -2164,16 +2179,16 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="11"/>
+        <v>88</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="I69" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J69" s="5" t="s">
         <v>39</v>
@@ -2183,13 +2198,13 @@
       <c r="M69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
+      <c r="B70" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
       <c r="I70" s="5" t="s">
         <v>53</v>
       </c>
@@ -2202,7 +2217,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I71" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J71" s="5" t="s">
         <v>11</v>
@@ -2213,16 +2228,16 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C72" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
+      <c r="C72" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
       <c r="I72" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J72" s="5" t="s">
         <v>39</v>
@@ -2248,10 +2263,10 @@
         <v>9</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
@@ -2259,21 +2274,21 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D74" s="11"/>
+        <v>116</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="5"/>
       <c r="E74" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="5"/>
       <c r="I74" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
@@ -2281,16 +2296,16 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75" s="11"/>
+        <v>118</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="I75" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J75" s="5" t="s">
         <v>11</v>
@@ -2302,16 +2317,80 @@
       <c r="M75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
+      <c r="B76" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F83" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="J4:M4"/>
@@ -2333,6 +2412,8 @@
     <mergeCell ref="B70:F70"/>
     <mergeCell ref="C72:F72"/>
     <mergeCell ref="B76:F76"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="B82:F82"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>